<commit_message>
some addition in schedual creation
</commit_message>
<xml_diff>
--- a/server/public/downloads/Schedule.xlsx
+++ b/server/public/downloads/Schedule.xlsx
@@ -55,19 +55,22 @@
     <t>Muhammad Abdullah</t>
   </si>
   <si>
+    <t>A22</t>
+  </si>
+  <si>
+    <t>CSF18M</t>
+  </si>
+  <si>
+    <t>Nimra Akram</t>
+  </si>
+  <si>
+    <t>B08</t>
+  </si>
+  <si>
     <t>08:15 - 09:19</t>
   </si>
   <si>
-    <t>CSF18M</t>
-  </si>
-  <si>
-    <t>Marriam Butt</t>
-  </si>
-  <si>
-    <t>A19</t>
-  </si>
-  <si>
-    <t>Sun Jun 19 2022 05:00:00 GMT+0500 (Pakistan Standard Time)</t>
+    <t>Wed Jun 15 2022 05:00:00 GMT+0500 (Pakistan Standard Time)</t>
   </si>
   <si>
     <t>Management Information Systems</t>
@@ -76,7 +79,13 @@
     <t>ITF18A</t>
   </si>
   <si>
-    <t>Mon Jun 20 2022 05:00:00 GMT+0500 (Pakistan Standard Time)</t>
+    <t>Muhammad Usman</t>
+  </si>
+  <si>
+    <t>B07</t>
+  </si>
+  <si>
+    <t>Tue Jun 21 2022 05:00:00 GMT+0500 (Pakistan Standard Time)</t>
   </si>
   <si>
     <t>Introduction to Parallel Programming</t>
@@ -85,22 +94,7 @@
     <t>ITF18M</t>
   </si>
   <si>
-    <t>Muhammad Mazhar</t>
-  </si>
-  <si>
-    <t>A20</t>
-  </si>
-  <si>
-    <t>Probability &amp; Statistics</t>
-  </si>
-  <si>
-    <t>SEF18A</t>
-  </si>
-  <si>
-    <t>A18</t>
-  </si>
-  <si>
-    <t>Wed Jun 15 2022 05:00:00 GMT+0500 (Pakistan Standard Time)</t>
+    <t>B09</t>
   </si>
 </sst>
 </file>
@@ -201,10 +195,10 @@
         <v>13</v>
       </c>
       <c r="D3" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="E3" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="F3" t="s">
         <v>11</v>
@@ -224,70 +218,50 @@
         <v>17</v>
       </c>
       <c r="E4" t="s">
-        <v>10</v>
+        <v>18</v>
       </c>
       <c r="F4" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B5" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C5" t="s">
-        <v>16</v>
+        <v>22</v>
       </c>
       <c r="D5" t="s">
-        <v>17</v>
+        <v>23</v>
       </c>
       <c r="E5" t="s">
-        <v>10</v>
+        <v>18</v>
       </c>
       <c r="F5" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
+        <v>25</v>
+      </c>
+      <c r="B6" t="s">
+        <v>26</v>
+      </c>
+      <c r="C6" t="s">
         <v>22</v>
       </c>
-      <c r="B6" t="s">
-        <v>23</v>
-      </c>
-      <c r="C6" t="s">
-        <v>24</v>
-      </c>
       <c r="D6" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="E6" t="s">
         <v>10</v>
       </c>
       <c r="F6" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="s">
-        <v>26</v>
-      </c>
-      <c r="B7" t="s">
-        <v>27</v>
-      </c>
-      <c r="C7" t="s">
         <v>24</v>
-      </c>
-      <c r="D7" t="s">
-        <v>28</v>
-      </c>
-      <c r="E7" t="s">
-        <v>10</v>
-      </c>
-      <c r="F7" t="s">
-        <v>29</v>
       </c>
     </row>
   </sheetData>

</xml_diff>